<commit_message>
br 1 by 1
</commit_message>
<xml_diff>
--- a/DQMF_table summary.xlsx
+++ b/DQMF_table summary.xlsx
@@ -379,7 +379,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -412,7 +412,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,17 +444,17 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H53" totalsRowShown="0">
   <autoFilter ref="A1:H53">
-    <filterColumn colId="4">
+    <filterColumn colId="1">
       <filters>
-        <filter val="etl, data quality, meta"/>
-        <filter val="etl, meta"/>
-        <filter val="meta"/>
-        <filter val="meta, etl"/>
+        <filter val="AuditDataCorrectionMapping"/>
+        <filter val="DQMF_BizRuleLookupMapping"/>
+        <filter val="DQMF_DataCorrectionMapping"/>
+        <filter val="ETL_PackageMapToSourceSystem"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState ref="A7:G37">
-    <sortCondition ref="E1:E53"/>
+  <sortState ref="A7:H37">
+    <sortCondition ref="C1:C53"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" name="schema_name"/>
@@ -736,7 +736,7 @@
   <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,27 +897,27 @@
       </c>
       <c r="H6"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="C7">
-        <v>8539</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
         <v>74</v>
       </c>
       <c r="E7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G7" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -968,7 +968,7 @@
       </c>
       <c r="H9"/>
     </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -989,73 +989,76 @@
       </c>
       <c r="H10"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="C11">
-        <v>477051</v>
+        <v>34</v>
       </c>
       <c r="D11" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="E11" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F11" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="G11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C12">
-        <v>131239</v>
+        <v>66</v>
       </c>
       <c r="D12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F12" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G12" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="C13">
-        <v>209</v>
+        <v>71</v>
       </c>
       <c r="D13" t="s">
         <v>74</v>
       </c>
       <c r="E13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F13" t="s">
         <v>92</v>
       </c>
       <c r="G13" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -1079,38 +1082,38 @@
       </c>
       <c r="H14"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="C15">
-        <v>78470</v>
+        <v>209</v>
       </c>
       <c r="D15" t="s">
         <v>74</v>
       </c>
       <c r="E15" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G15" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C16">
-        <v>50282</v>
+        <v>375</v>
       </c>
       <c r="D16" t="s">
         <v>74</v>
@@ -1119,10 +1122,13 @@
         <v>84</v>
       </c>
       <c r="F16" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G16" t="s">
-        <v>113</v>
+        <v>108</v>
+      </c>
+      <c r="H16" s="1">
+        <v>41324.647351701387</v>
       </c>
     </row>
     <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1149,30 +1155,30 @@
       </c>
       <c r="H17"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18">
-        <v>23827</v>
+        <v>1226</v>
       </c>
       <c r="D18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E18" t="s">
         <v>84</v>
       </c>
       <c r="F18" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G18" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -1196,15 +1202,15 @@
       </c>
       <c r="H19"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C20">
-        <v>3902</v>
+        <v>3021</v>
       </c>
       <c r="D20" t="s">
         <v>74</v>
@@ -1213,16 +1219,13 @@
         <v>84</v>
       </c>
       <c r="F20" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="G20" t="s">
-        <v>87</v>
-      </c>
-      <c r="H20" s="1">
-        <v>42544.7300034375</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -1245,15 +1248,15 @@
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C22">
-        <v>3021</v>
+        <v>3902</v>
       </c>
       <c r="D22" t="s">
         <v>74</v>
@@ -1262,33 +1265,36 @@
         <v>84</v>
       </c>
       <c r="F22" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="G22" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="H22" s="1">
+        <v>42544.7300034375</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="C23">
-        <v>1226</v>
+        <v>8539</v>
       </c>
       <c r="D23" t="s">
         <v>74</v>
       </c>
       <c r="E23" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="F23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G23" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1387,41 +1393,38 @@
       </c>
       <c r="H27"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C28">
-        <v>375</v>
+        <v>23827</v>
       </c>
       <c r="D28" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E28" t="s">
         <v>84</v>
       </c>
       <c r="F28" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G28" t="s">
-        <v>108</v>
-      </c>
-      <c r="H28" s="1">
-        <v>41324.647351701387</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>2</v>
       </c>
       <c r="B29" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C29">
-        <v>71</v>
+        <v>50282</v>
       </c>
       <c r="D29" t="s">
         <v>74</v>
@@ -1430,10 +1433,10 @@
         <v>84</v>
       </c>
       <c r="F29" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="G29" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1460,7 +1463,7 @@
       </c>
       <c r="H30"/>
     </row>
-    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -1508,15 +1511,15 @@
       </c>
       <c r="H32"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C33">
-        <v>66</v>
+        <v>78470</v>
       </c>
       <c r="D33" t="s">
         <v>74</v>
@@ -1528,10 +1531,10 @@
         <v>94</v>
       </c>
       <c r="G33" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>2</v>
       </c>
@@ -1557,27 +1560,27 @@
         <v>42544.745267326391</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C35">
-        <v>34</v>
+        <v>131239</v>
       </c>
       <c r="D35" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E35" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F35" t="s">
         <v>92</v>
       </c>
       <c r="G35" t="s">
-        <v>98</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1604,27 +1607,24 @@
       </c>
       <c r="H36"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>2</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="C37">
-        <v>15</v>
+        <v>477051</v>
       </c>
       <c r="D37" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="E37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F37" t="s">
-        <v>94</v>
-      </c>
-      <c r="G37" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">

</xml_diff>